<commit_message>
ajuste de la operacion reductions y manejo de actions
</commit_message>
<xml_diff>
--- a/ProyectoConsola/ProyectoConsola/bin/Debug/net8.0/estados.xlsx
+++ b/ProyectoConsola/ProyectoConsola/bin/Debug/net8.0/estados.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="355">
   <si>
     <t>Estado actual</t>
   </si>
@@ -428,7 +428,7 @@
     <t>string_constant</t>
   </si>
   <si>
-    <t>'"' str'"'</t>
+    <t>'"' str '"'</t>
   </si>
   <si>
     <t>'"' / 0</t>
@@ -683,7 +683,7 @@
     <t>Estado: 48</t>
   </si>
   <si>
-    <t>str'"' / 1</t>
+    <t>str / 1</t>
   </si>
   <si>
     <t>Estado: 49</t>
@@ -785,7 +785,7 @@
     <t>argument_list_ext</t>
   </si>
   <si>
-    <t>',' &lt;expression&gt;&lt;argument_list_ext&gt;</t>
+    <t>',' &lt;expression&gt; &lt;argument_list_ext&gt;</t>
   </si>
   <si>
     <t>',' / 0</t>
@@ -866,6 +866,9 @@
     <t>Estado: 91</t>
   </si>
   <si>
+    <t>'"' / 2</t>
+  </si>
+  <si>
     <t>Estado: 92</t>
   </si>
   <si>
@@ -926,9 +929,6 @@
     <t>Estado: 107</t>
   </si>
   <si>
-    <t>&lt;expression&gt;&lt;argument_list_ext&gt; / 1</t>
-  </si>
-  <si>
     <t>Estado: 108</t>
   </si>
   <si>
@@ -968,16 +968,19 @@
     <t>Estado: 116</t>
   </si>
   <si>
+    <t>Estado: 117</t>
+  </si>
+  <si>
     <t>E.O.P. / 6</t>
   </si>
   <si>
-    <t>Estado: 117</t>
+    <t>Estado: 118</t>
   </si>
   <si>
     <t>&lt;block&gt; / 6</t>
   </si>
   <si>
-    <t>Estado: 118</t>
+    <t>Estado: 119</t>
   </si>
   <si>
     <t>&lt;parameter_list_ext&gt; / 3</t>
@@ -989,9 +992,6 @@
     <t>',' identifier ':' &lt;type&gt; &lt;parameter_list_ext&gt;</t>
   </si>
   <si>
-    <t>Estado: 119</t>
-  </si>
-  <si>
     <t>Estado: 120</t>
   </si>
   <si>
@@ -1013,18 +1013,21 @@
     <t>Estado: 126</t>
   </si>
   <si>
+    <t>&lt;argument_list_ext&gt; / 2</t>
+  </si>
+  <si>
     <t>Estado: 127</t>
   </si>
   <si>
     <t>Estado: 128</t>
   </si>
   <si>
+    <t>Estado: 129</t>
+  </si>
+  <si>
     <t>';' / 7</t>
   </si>
   <si>
-    <t>Estado: 129</t>
-  </si>
-  <si>
     <t>Estado: 130</t>
   </si>
   <si>
@@ -1049,25 +1052,31 @@
     <t>Estado: 137</t>
   </si>
   <si>
+    <t>Estado: 138</t>
+  </si>
+  <si>
+    <t>Estado: 139</t>
+  </si>
+  <si>
     <t>E.O.P. / 8</t>
   </si>
   <si>
-    <t>Estado: 138</t>
-  </si>
-  <si>
-    <t>Estado: 139</t>
-  </si>
-  <si>
     <t>Estado: 140</t>
   </si>
   <si>
     <t>Estado: 141</t>
   </si>
   <si>
+    <t>Estado: 142</t>
+  </si>
+  <si>
+    <t>Estado: 143</t>
+  </si>
+  <si>
     <t>&lt;parameter_list_ext&gt; / 4</t>
   </si>
   <si>
-    <t>Estado: 142</t>
+    <t>Estado: 144</t>
   </si>
 </sst>
 </file>
@@ -1114,7 +1123,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr codeName=""/>
-  <dimension ref="A1:D756"/>
+  <dimension ref="A1:D774"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -5975,7 +5984,7 @@
         <v>138</v>
       </c>
       <c r="C498" s="0" t="s">
-        <v>53</v>
+        <v>284</v>
       </c>
       <c r="D498" s="0" t="s">
         <v>124</v>
@@ -5983,7 +5992,7 @@
     </row>
     <row r="500">
       <c r="A500" s="0" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="501">
@@ -6170,7 +6179,7 @@
     </row>
     <row r="515">
       <c r="A515" s="0" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="516">
@@ -6203,7 +6212,7 @@
     </row>
     <row r="519">
       <c r="A519" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="520">
@@ -6236,7 +6245,7 @@
     </row>
     <row r="523">
       <c r="A523" s="0" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="524">
@@ -6247,7 +6256,7 @@
         <v>30</v>
       </c>
       <c r="C524" s="0" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="D524" s="0" t="s">
         <v>32</v>
@@ -6269,7 +6278,7 @@
     </row>
     <row r="527">
       <c r="A527" s="0" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
     </row>
     <row r="528">
@@ -6280,7 +6289,7 @@
         <v>36</v>
       </c>
       <c r="C528" s="0" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="D528" s="0" t="s">
         <v>32</v>
@@ -6288,7 +6297,7 @@
     </row>
     <row r="530">
       <c r="A530" s="0" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="531">
@@ -6299,7 +6308,7 @@
         <v>161</v>
       </c>
       <c r="C531" s="0" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="D531" s="0" t="s">
         <v>162</v>
@@ -6363,7 +6372,7 @@
     </row>
     <row r="537">
       <c r="A537" s="0" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
     </row>
     <row r="538">
@@ -6382,7 +6391,7 @@
     </row>
     <row r="540">
       <c r="A540" s="0" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="541">
@@ -6555,7 +6564,7 @@
     </row>
     <row r="554">
       <c r="A554" s="0" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="555">
@@ -6742,7 +6751,7 @@
     </row>
     <row r="569">
       <c r="A569" s="0" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
     </row>
     <row r="570">
@@ -6761,7 +6770,7 @@
     </row>
     <row r="572">
       <c r="A572" s="0" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
     <row r="573">
@@ -6780,7 +6789,7 @@
     </row>
     <row r="575">
       <c r="A575" s="0" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
     </row>
     <row r="576">
@@ -6953,7 +6962,7 @@
     </row>
     <row r="589">
       <c r="A589" s="0" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
     </row>
     <row r="590">
@@ -6972,7 +6981,7 @@
     </row>
     <row r="592">
       <c r="A592" s="0" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
     </row>
     <row r="593">
@@ -6983,7 +6992,7 @@
         <v>79</v>
       </c>
       <c r="C593" s="0" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="D593" s="0" t="s">
         <v>59</v>
@@ -6997,7 +7006,7 @@
         <v>79</v>
       </c>
       <c r="C594" s="0" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="D594" s="0" t="s">
         <v>88</v>
@@ -7005,7 +7014,7 @@
     </row>
     <row r="596">
       <c r="A596" s="0" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
     </row>
     <row r="597">
@@ -7024,7 +7033,7 @@
     </row>
     <row r="599">
       <c r="A599" s="0" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row r="600">
@@ -7035,584 +7044,584 @@
         <v>257</v>
       </c>
       <c r="C600" s="0" t="s">
-        <v>304</v>
+        <v>108</v>
       </c>
       <c r="D600" s="0" t="s">
         <v>162</v>
       </c>
     </row>
+    <row r="601">
+      <c r="A601" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="B601" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="C601" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="D601" s="0" t="s">
+        <v>175</v>
+      </c>
+    </row>
     <row r="602">
       <c r="A602" s="0" t="s">
-        <v>305</v>
+        <v>113</v>
+      </c>
+      <c r="B602" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="C602" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="D602" s="0" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="603">
       <c r="A603" s="0" t="s">
-        <v>68</v>
+        <v>117</v>
       </c>
       <c r="B603" s="0" t="s">
-        <v>69</v>
+        <v>118</v>
       </c>
       <c r="C603" s="0" t="s">
-        <v>306</v>
+        <v>119</v>
       </c>
       <c r="D603" s="0" t="s">
-        <v>59</v>
+        <v>120</v>
       </c>
     </row>
     <row r="604">
       <c r="A604" s="0" t="s">
-        <v>68</v>
+        <v>121</v>
       </c>
       <c r="B604" s="0" t="s">
-        <v>69</v>
+        <v>122</v>
       </c>
       <c r="C604" s="0" t="s">
-        <v>306</v>
+        <v>123</v>
       </c>
       <c r="D604" s="0" t="s">
-        <v>88</v>
+        <v>124</v>
       </c>
     </row>
     <row r="605">
       <c r="A605" s="0" t="s">
-        <v>307</v>
+        <v>121</v>
       </c>
       <c r="B605" s="0" t="s">
-        <v>308</v>
+        <v>125</v>
       </c>
       <c r="C605" s="0" t="s">
-        <v>309</v>
+        <v>65</v>
       </c>
       <c r="D605" s="0" t="s">
-        <v>88</v>
+        <v>124</v>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="B606" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="C606" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="D606" s="0" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="607">
       <c r="A607" s="0" t="s">
-        <v>310</v>
+        <v>121</v>
+      </c>
+      <c r="B607" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="C607" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="D607" s="0" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="608">
       <c r="A608" s="0" t="s">
-        <v>180</v>
+        <v>130</v>
       </c>
       <c r="B608" s="0" t="s">
-        <v>181</v>
+        <v>131</v>
       </c>
       <c r="C608" s="0" t="s">
-        <v>53</v>
+        <v>132</v>
       </c>
       <c r="D608" s="0" t="s">
-        <v>112</v>
+        <v>124</v>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="B609" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="C609" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="D609" s="0" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="610">
       <c r="A610" s="0" t="s">
-        <v>311</v>
+        <v>121</v>
+      </c>
+      <c r="B610" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="C610" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="D610" s="0" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="611">
       <c r="A611" s="0" t="s">
-        <v>113</v>
+        <v>137</v>
       </c>
       <c r="B611" s="0" t="s">
-        <v>114</v>
+        <v>138</v>
       </c>
       <c r="C611" s="0" t="s">
-        <v>164</v>
+        <v>139</v>
       </c>
       <c r="D611" s="0" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
     </row>
     <row r="613">
       <c r="A613" s="0" t="s">
-        <v>312</v>
+        <v>305</v>
       </c>
     </row>
     <row r="614">
       <c r="A614" s="0" t="s">
-        <v>117</v>
+        <v>68</v>
       </c>
       <c r="B614" s="0" t="s">
-        <v>118</v>
+        <v>69</v>
       </c>
       <c r="C614" s="0" t="s">
-        <v>164</v>
+        <v>306</v>
       </c>
       <c r="D614" s="0" t="s">
-        <v>120</v>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="B615" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="C615" s="0" t="s">
+        <v>306</v>
+      </c>
+      <c r="D615" s="0" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="616">
       <c r="A616" s="0" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="617">
-      <c r="A617" s="0" t="s">
-        <v>121</v>
-      </c>
-      <c r="B617" s="0" t="s">
-        <v>122</v>
-      </c>
-      <c r="C617" s="0" t="s">
-        <v>164</v>
-      </c>
-      <c r="D617" s="0" t="s">
-        <v>124</v>
+        <v>307</v>
+      </c>
+      <c r="B616" s="0" t="s">
+        <v>308</v>
+      </c>
+      <c r="C616" s="0" t="s">
+        <v>309</v>
+      </c>
+      <c r="D616" s="0" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" s="0" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="619">
       <c r="A619" s="0" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="620">
-      <c r="A620" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="B620" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="C620" s="0" t="s">
-        <v>301</v>
-      </c>
-      <c r="D620" s="0" t="s">
-        <v>59</v>
+        <v>180</v>
+      </c>
+      <c r="B619" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="C619" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="D619" s="0" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="621">
       <c r="A621" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="B621" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="C621" s="0" t="s">
-        <v>301</v>
-      </c>
-      <c r="D621" s="0" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="623">
-      <c r="A623" s="0" t="s">
-        <v>315</v>
+        <v>311</v>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="B622" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="C622" s="0" t="s">
+        <v>164</v>
+      </c>
+      <c r="D622" s="0" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="624">
       <c r="A624" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="B624" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="C624" s="0" t="s">
-        <v>301</v>
-      </c>
-      <c r="D624" s="0" t="s">
-        <v>59</v>
+        <v>312</v>
       </c>
     </row>
     <row r="625">
       <c r="A625" s="0" t="s">
-        <v>82</v>
+        <v>117</v>
       </c>
       <c r="B625" s="0" t="s">
-        <v>83</v>
+        <v>118</v>
       </c>
       <c r="C625" s="0" t="s">
-        <v>301</v>
+        <v>164</v>
       </c>
       <c r="D625" s="0" t="s">
-        <v>88</v>
+        <v>120</v>
       </c>
     </row>
     <row r="627">
       <c r="A627" s="0" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="628">
       <c r="A628" s="0" t="s">
-        <v>82</v>
+        <v>121</v>
       </c>
       <c r="B628" s="0" t="s">
-        <v>85</v>
+        <v>122</v>
       </c>
       <c r="C628" s="0" t="s">
-        <v>301</v>
+        <v>164</v>
       </c>
       <c r="D628" s="0" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="629">
-      <c r="A629" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="B629" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="C629" s="0" t="s">
-        <v>301</v>
-      </c>
-      <c r="D629" s="0" t="s">
-        <v>88</v>
+        <v>124</v>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" s="0" t="s">
+        <v>314</v>
       </c>
     </row>
     <row r="631">
       <c r="A631" s="0" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="632">
-      <c r="A632" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="B632" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="C632" s="0" t="s">
-        <v>318</v>
-      </c>
-      <c r="D632" s="0" t="s">
-        <v>32</v>
+        <v>137</v>
+      </c>
+      <c r="B631" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="C631" s="0" t="s">
+        <v>164</v>
+      </c>
+      <c r="D631" s="0" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" s="0" t="s">
+        <v>315</v>
       </c>
     </row>
     <row r="634">
       <c r="A634" s="0" t="s">
-        <v>319</v>
+        <v>73</v>
+      </c>
+      <c r="B634" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="C634" s="0" t="s">
+        <v>302</v>
+      </c>
+      <c r="D634" s="0" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="635">
       <c r="A635" s="0" t="s">
-        <v>35</v>
+        <v>73</v>
       </c>
       <c r="B635" s="0" t="s">
-        <v>36</v>
+        <v>74</v>
       </c>
       <c r="C635" s="0" t="s">
-        <v>320</v>
+        <v>302</v>
       </c>
       <c r="D635" s="0" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="636">
-      <c r="A636" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="B636" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="C636" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="D636" s="0" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="637">
       <c r="A637" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="B637" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="C637" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="D637" s="0" t="s">
-        <v>28</v>
+        <v>316</v>
       </c>
     </row>
     <row r="638">
       <c r="A638" s="0" t="s">
-        <v>29</v>
+        <v>82</v>
       </c>
       <c r="B638" s="0" t="s">
-        <v>30</v>
+        <v>83</v>
       </c>
       <c r="C638" s="0" t="s">
-        <v>31</v>
+        <v>302</v>
       </c>
       <c r="D638" s="0" t="s">
-        <v>32</v>
+        <v>59</v>
       </c>
     </row>
     <row r="639">
       <c r="A639" s="0" t="s">
-        <v>25</v>
+        <v>82</v>
       </c>
       <c r="B639" s="0" t="s">
-        <v>33</v>
+        <v>83</v>
       </c>
       <c r="C639" s="0" t="s">
-        <v>34</v>
+        <v>302</v>
       </c>
       <c r="D639" s="0" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="640">
-      <c r="A640" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="B640" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="C640" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="D640" s="0" t="s">
-        <v>32</v>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" s="0" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="642">
       <c r="A642" s="0" t="s">
-        <v>321</v>
+        <v>82</v>
+      </c>
+      <c r="B642" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="C642" s="0" t="s">
+        <v>302</v>
+      </c>
+      <c r="D642" s="0" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="643">
       <c r="A643" s="0" t="s">
-        <v>160</v>
+        <v>82</v>
       </c>
       <c r="B643" s="0" t="s">
-        <v>161</v>
+        <v>85</v>
       </c>
       <c r="C643" s="0" t="s">
-        <v>322</v>
+        <v>302</v>
       </c>
       <c r="D643" s="0" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="644">
-      <c r="A644" s="0" t="s">
-        <v>323</v>
-      </c>
-      <c r="B644" s="0" t="s">
-        <v>324</v>
-      </c>
-      <c r="C644" s="0" t="s">
-        <v>258</v>
-      </c>
-      <c r="D644" s="0" t="s">
-        <v>162</v>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" s="0" t="s">
+        <v>318</v>
       </c>
     </row>
     <row r="646">
       <c r="A646" s="0" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="647">
-      <c r="A647" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="B647" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="C647" s="0" t="s">
-        <v>164</v>
-      </c>
-      <c r="D647" s="0" t="s">
-        <v>88</v>
+        <v>29</v>
+      </c>
+      <c r="B646" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="C646" s="0" t="s">
+        <v>319</v>
+      </c>
+      <c r="D646" s="0" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" s="0" t="s">
+        <v>320</v>
       </c>
     </row>
     <row r="649">
       <c r="A649" s="0" t="s">
-        <v>326</v>
+        <v>35</v>
+      </c>
+      <c r="B649" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="C649" s="0" t="s">
+        <v>321</v>
+      </c>
+      <c r="D649" s="0" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="650">
       <c r="A650" s="0" t="s">
-        <v>78</v>
+        <v>21</v>
       </c>
       <c r="B650" s="0" t="s">
-        <v>79</v>
+        <v>22</v>
       </c>
       <c r="C650" s="0" t="s">
-        <v>253</v>
+        <v>23</v>
       </c>
       <c r="D650" s="0" t="s">
         <v>88</v>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B651" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C651" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="D651" s="0" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="652">
       <c r="A652" s="0" t="s">
-        <v>327</v>
+        <v>29</v>
+      </c>
+      <c r="B652" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="C652" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D652" s="0" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="653">
       <c r="A653" s="0" t="s">
-        <v>68</v>
+        <v>25</v>
       </c>
       <c r="B653" s="0" t="s">
-        <v>69</v>
+        <v>33</v>
       </c>
       <c r="C653" s="0" t="s">
-        <v>260</v>
+        <v>34</v>
       </c>
       <c r="D653" s="0" t="s">
-        <v>88</v>
+        <v>28</v>
       </c>
     </row>
     <row r="654">
       <c r="A654" s="0" t="s">
-        <v>60</v>
+        <v>35</v>
       </c>
       <c r="B654" s="0" t="s">
-        <v>61</v>
+        <v>36</v>
       </c>
       <c r="C654" s="0" t="s">
-        <v>62</v>
+        <v>37</v>
       </c>
       <c r="D654" s="0" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="655">
-      <c r="A655" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="B655" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="C655" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="D655" s="0" t="s">
-        <v>261</v>
+        <v>32</v>
       </c>
     </row>
     <row r="656">
       <c r="A656" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="B656" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="C656" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="D656" s="0" t="s">
-        <v>261</v>
+        <v>322</v>
       </c>
     </row>
     <row r="657">
       <c r="A657" s="0" t="s">
-        <v>68</v>
+        <v>160</v>
       </c>
       <c r="B657" s="0" t="s">
-        <v>69</v>
+        <v>161</v>
       </c>
       <c r="C657" s="0" t="s">
-        <v>70</v>
+        <v>323</v>
       </c>
       <c r="D657" s="0" t="s">
-        <v>261</v>
+        <v>162</v>
       </c>
     </row>
     <row r="658">
       <c r="A658" s="0" t="s">
-        <v>60</v>
+        <v>324</v>
       </c>
       <c r="B658" s="0" t="s">
-        <v>71</v>
+        <v>325</v>
       </c>
       <c r="C658" s="0" t="s">
-        <v>72</v>
+        <v>258</v>
       </c>
       <c r="D658" s="0" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="659">
-      <c r="A659" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="B659" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="C659" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="D659" s="0" t="s">
-        <v>261</v>
+        <v>162</v>
       </c>
     </row>
     <row r="660">
       <c r="A660" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="B660" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="C660" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="D660" s="0" t="s">
-        <v>261</v>
+        <v>326</v>
       </c>
     </row>
     <row r="661">
       <c r="A661" s="0" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="B661" s="0" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="C661" s="0" t="s">
-        <v>65</v>
+        <v>164</v>
       </c>
       <c r="D661" s="0" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="662">
-      <c r="A662" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="B662" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="C662" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="D662" s="0" t="s">
-        <v>261</v>
+        <v>88</v>
       </c>
     </row>
     <row r="663">
       <c r="A663" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="B663" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="C663" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="D663" s="0" t="s">
-        <v>261</v>
+        <v>327</v>
       </c>
     </row>
     <row r="664">
       <c r="A664" s="0" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B664" s="0" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="C664" s="0" t="s">
-        <v>86</v>
+        <v>253</v>
       </c>
       <c r="D664" s="0" t="s">
-        <v>261</v>
+        <v>88</v>
       </c>
     </row>
     <row r="666">
@@ -7622,10 +7631,10 @@
     </row>
     <row r="667">
       <c r="A667" s="0" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B667" s="0" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C667" s="0" t="s">
         <v>260</v>
@@ -7645,7 +7654,7 @@
         <v>62</v>
       </c>
       <c r="D668" s="0" t="s">
-        <v>88</v>
+        <v>261</v>
       </c>
     </row>
     <row r="669">
@@ -7659,7 +7668,7 @@
         <v>65</v>
       </c>
       <c r="D669" s="0" t="s">
-        <v>88</v>
+        <v>261</v>
       </c>
     </row>
     <row r="670">
@@ -7673,7 +7682,7 @@
         <v>67</v>
       </c>
       <c r="D670" s="0" t="s">
-        <v>88</v>
+        <v>261</v>
       </c>
     </row>
     <row r="671">
@@ -7687,7 +7696,7 @@
         <v>70</v>
       </c>
       <c r="D671" s="0" t="s">
-        <v>88</v>
+        <v>261</v>
       </c>
     </row>
     <row r="672">
@@ -7701,7 +7710,7 @@
         <v>72</v>
       </c>
       <c r="D672" s="0" t="s">
-        <v>88</v>
+        <v>261</v>
       </c>
     </row>
     <row r="673">
@@ -7715,7 +7724,7 @@
         <v>75</v>
       </c>
       <c r="D673" s="0" t="s">
-        <v>88</v>
+        <v>261</v>
       </c>
     </row>
     <row r="674">
@@ -7729,7 +7738,7 @@
         <v>77</v>
       </c>
       <c r="D674" s="0" t="s">
-        <v>88</v>
+        <v>261</v>
       </c>
     </row>
     <row r="675">
@@ -7743,7 +7752,7 @@
         <v>65</v>
       </c>
       <c r="D675" s="0" t="s">
-        <v>88</v>
+        <v>261</v>
       </c>
     </row>
     <row r="676">
@@ -7757,7 +7766,7 @@
         <v>81</v>
       </c>
       <c r="D676" s="0" t="s">
-        <v>88</v>
+        <v>261</v>
       </c>
     </row>
     <row r="677">
@@ -7771,7 +7780,7 @@
         <v>84</v>
       </c>
       <c r="D677" s="0" t="s">
-        <v>88</v>
+        <v>261</v>
       </c>
     </row>
     <row r="678">
@@ -7785,7 +7794,7 @@
         <v>86</v>
       </c>
       <c r="D678" s="0" t="s">
-        <v>88</v>
+        <v>261</v>
       </c>
     </row>
     <row r="680">
@@ -7795,322 +7804,391 @@
     </row>
     <row r="681">
       <c r="A681" s="0" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="B681" s="0" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="C681" s="0" t="s">
-        <v>253</v>
+        <v>260</v>
       </c>
       <c r="D681" s="0" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="B682" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="C682" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="D682" s="0" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="683">
       <c r="A683" s="0" t="s">
-        <v>330</v>
+        <v>63</v>
+      </c>
+      <c r="B683" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C683" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="D683" s="0" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="684">
       <c r="A684" s="0" t="s">
-        <v>82</v>
+        <v>60</v>
       </c>
       <c r="B684" s="0" t="s">
-        <v>85</v>
+        <v>66</v>
       </c>
       <c r="C684" s="0" t="s">
-        <v>253</v>
+        <v>67</v>
       </c>
       <c r="D684" s="0" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="B685" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="C685" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="D685" s="0" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="686">
       <c r="A686" s="0" t="s">
-        <v>331</v>
+        <v>60</v>
+      </c>
+      <c r="B686" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="C686" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="D686" s="0" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="687">
       <c r="A687" s="0" t="s">
-        <v>256</v>
+        <v>73</v>
       </c>
       <c r="B687" s="0" t="s">
-        <v>257</v>
+        <v>74</v>
       </c>
       <c r="C687" s="0" t="s">
-        <v>53</v>
+        <v>75</v>
       </c>
       <c r="D687" s="0" t="s">
-        <v>162</v>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="B688" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="C688" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="D688" s="0" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="689">
       <c r="A689" s="0" t="s">
-        <v>332</v>
+        <v>78</v>
+      </c>
+      <c r="B689" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="C689" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="D689" s="0" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="690">
       <c r="A690" s="0" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="B690" s="0" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="C690" s="0" t="s">
-        <v>51</v>
+        <v>81</v>
       </c>
       <c r="D690" s="0" t="s">
-        <v>59</v>
+        <v>88</v>
       </c>
     </row>
     <row r="691">
       <c r="A691" s="0" t="s">
-        <v>68</v>
+        <v>82</v>
       </c>
       <c r="B691" s="0" t="s">
-        <v>69</v>
+        <v>83</v>
       </c>
       <c r="C691" s="0" t="s">
-        <v>51</v>
+        <v>84</v>
       </c>
       <c r="D691" s="0" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="693">
-      <c r="A693" s="0" t="s">
-        <v>333</v>
+    <row r="692">
+      <c r="A692" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="B692" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="C692" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="D692" s="0" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="694">
       <c r="A694" s="0" t="s">
-        <v>307</v>
-      </c>
-      <c r="B694" s="0" t="s">
-        <v>308</v>
-      </c>
-      <c r="C694" s="0" t="s">
-        <v>167</v>
-      </c>
-      <c r="D694" s="0" t="s">
-        <v>88</v>
+        <v>330</v>
       </c>
     </row>
     <row r="695">
       <c r="A695" s="0" t="s">
-        <v>60</v>
+        <v>82</v>
       </c>
       <c r="B695" s="0" t="s">
-        <v>61</v>
+        <v>83</v>
       </c>
       <c r="C695" s="0" t="s">
-        <v>62</v>
+        <v>253</v>
       </c>
       <c r="D695" s="0" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="696">
-      <c r="A696" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="B696" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="C696" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="D696" s="0" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="697">
       <c r="A697" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="B697" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="C697" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="D697" s="0" t="s">
-        <v>88</v>
+        <v>331</v>
       </c>
     </row>
     <row r="698">
       <c r="A698" s="0" t="s">
-        <v>68</v>
+        <v>82</v>
       </c>
       <c r="B698" s="0" t="s">
-        <v>69</v>
+        <v>85</v>
       </c>
       <c r="C698" s="0" t="s">
-        <v>70</v>
+        <v>253</v>
       </c>
       <c r="D698" s="0" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="699">
-      <c r="A699" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="B699" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="C699" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="D699" s="0" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="700">
       <c r="A700" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="B700" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="C700" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="D700" s="0" t="s">
-        <v>88</v>
+        <v>332</v>
       </c>
     </row>
     <row r="701">
       <c r="A701" s="0" t="s">
-        <v>60</v>
+        <v>256</v>
       </c>
       <c r="B701" s="0" t="s">
-        <v>76</v>
+        <v>257</v>
       </c>
       <c r="C701" s="0" t="s">
-        <v>77</v>
+        <v>333</v>
       </c>
       <c r="D701" s="0" t="s">
-        <v>88</v>
+        <v>162</v>
       </c>
     </row>
     <row r="702">
       <c r="A702" s="0" t="s">
-        <v>78</v>
+        <v>256</v>
       </c>
       <c r="B702" s="0" t="s">
-        <v>79</v>
+        <v>257</v>
       </c>
       <c r="C702" s="0" t="s">
-        <v>65</v>
+        <v>258</v>
       </c>
       <c r="D702" s="0" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="703">
-      <c r="A703" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="B703" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="C703" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="D703" s="0" t="s">
-        <v>88</v>
+        <v>162</v>
       </c>
     </row>
     <row r="704">
       <c r="A704" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="B704" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="C704" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="D704" s="0" t="s">
-        <v>88</v>
+        <v>334</v>
       </c>
     </row>
     <row r="705">
       <c r="A705" s="0" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="B705" s="0" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="C705" s="0" t="s">
-        <v>86</v>
+        <v>51</v>
       </c>
       <c r="D705" s="0" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="707">
-      <c r="A707" s="0" t="s">
-        <v>334</v>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="B706" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="C706" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="D706" s="0" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="708">
       <c r="A708" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="B708" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="C708" s="0" t="s">
         <v>335</v>
       </c>
-      <c r="D708" s="0" t="s">
-        <v>32</v>
+    </row>
+    <row r="709">
+      <c r="A709" s="0" t="s">
+        <v>307</v>
+      </c>
+      <c r="B709" s="0" t="s">
+        <v>308</v>
+      </c>
+      <c r="C709" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="D709" s="0" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="710">
       <c r="A710" s="0" t="s">
-        <v>336</v>
+        <v>60</v>
+      </c>
+      <c r="B710" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="C710" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="D710" s="0" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="711">
       <c r="A711" s="0" t="s">
-        <v>160</v>
+        <v>63</v>
       </c>
       <c r="B711" s="0" t="s">
-        <v>161</v>
+        <v>64</v>
       </c>
       <c r="C711" s="0" t="s">
-        <v>301</v>
+        <v>65</v>
       </c>
       <c r="D711" s="0" t="s">
-        <v>162</v>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="B712" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="C712" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="D712" s="0" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="713">
       <c r="A713" s="0" t="s">
-        <v>337</v>
+        <v>68</v>
+      </c>
+      <c r="B713" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="C713" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="D713" s="0" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="714">
       <c r="A714" s="0" t="s">
-        <v>323</v>
+        <v>60</v>
       </c>
       <c r="B714" s="0" t="s">
-        <v>324</v>
+        <v>71</v>
       </c>
       <c r="C714" s="0" t="s">
-        <v>16</v>
+        <v>72</v>
       </c>
       <c r="D714" s="0" t="s">
-        <v>162</v>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="B715" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="C715" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="D715" s="0" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="716">
       <c r="A716" s="0" t="s">
-        <v>338</v>
+        <v>60</v>
+      </c>
+      <c r="B716" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="C716" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="D716" s="0" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="717">
@@ -8121,173 +8199,196 @@
         <v>79</v>
       </c>
       <c r="C717" s="0" t="s">
-        <v>301</v>
+        <v>65</v>
       </c>
       <c r="D717" s="0" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="B718" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="C718" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="D718" s="0" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="719">
       <c r="A719" s="0" t="s">
-        <v>339</v>
+        <v>82</v>
+      </c>
+      <c r="B719" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="C719" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="D719" s="0" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="720">
       <c r="A720" s="0" t="s">
-        <v>68</v>
+        <v>82</v>
       </c>
       <c r="B720" s="0" t="s">
-        <v>69</v>
+        <v>85</v>
       </c>
       <c r="C720" s="0" t="s">
-        <v>306</v>
+        <v>86</v>
       </c>
       <c r="D720" s="0" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="721">
-      <c r="A721" s="0" t="s">
-        <v>307</v>
-      </c>
-      <c r="B721" s="0" t="s">
-        <v>308</v>
-      </c>
-      <c r="C721" s="0" t="s">
-        <v>309</v>
-      </c>
-      <c r="D721" s="0" t="s">
-        <v>88</v>
+    <row r="722">
+      <c r="A722" s="0" t="s">
+        <v>336</v>
       </c>
     </row>
     <row r="723">
       <c r="A723" s="0" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="724">
-      <c r="A724" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="B724" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="C724" s="0" t="s">
-        <v>301</v>
-      </c>
-      <c r="D724" s="0" t="s">
-        <v>88</v>
+        <v>35</v>
+      </c>
+      <c r="B723" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="C723" s="0" t="s">
+        <v>337</v>
+      </c>
+      <c r="D723" s="0" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" s="0" t="s">
+        <v>338</v>
       </c>
     </row>
     <row r="726">
       <c r="A726" s="0" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="727">
-      <c r="A727" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="B727" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="C727" s="0" t="s">
-        <v>301</v>
-      </c>
-      <c r="D727" s="0" t="s">
-        <v>88</v>
+        <v>160</v>
+      </c>
+      <c r="B726" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="C726" s="0" t="s">
+        <v>302</v>
+      </c>
+      <c r="D726" s="0" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" s="0" t="s">
+        <v>339</v>
       </c>
     </row>
     <row r="729">
       <c r="A729" s="0" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="730">
-      <c r="A730" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="B730" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="C730" s="0" t="s">
-        <v>301</v>
-      </c>
-      <c r="D730" s="0" t="s">
-        <v>88</v>
+        <v>324</v>
+      </c>
+      <c r="B729" s="0" t="s">
+        <v>325</v>
+      </c>
+      <c r="C729" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D729" s="0" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" s="0" t="s">
+        <v>340</v>
       </c>
     </row>
     <row r="732">
       <c r="A732" s="0" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="733">
-      <c r="A733" s="0" t="s">
-        <v>307</v>
-      </c>
-      <c r="B733" s="0" t="s">
-        <v>308</v>
-      </c>
-      <c r="C733" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="D733" s="0" t="s">
-        <v>88</v>
+        <v>78</v>
+      </c>
+      <c r="B732" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="C732" s="0" t="s">
+        <v>302</v>
+      </c>
+      <c r="D732" s="0" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" s="0" t="s">
+        <v>341</v>
       </c>
     </row>
     <row r="735">
       <c r="A735" s="0" t="s">
-        <v>344</v>
+        <v>68</v>
+      </c>
+      <c r="B735" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="C735" s="0" t="s">
+        <v>306</v>
+      </c>
+      <c r="D735" s="0" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="736">
       <c r="A736" s="0" t="s">
-        <v>35</v>
+        <v>307</v>
       </c>
       <c r="B736" s="0" t="s">
-        <v>36</v>
+        <v>308</v>
       </c>
       <c r="C736" s="0" t="s">
-        <v>345</v>
+        <v>309</v>
       </c>
       <c r="D736" s="0" t="s">
-        <v>32</v>
+        <v>88</v>
       </c>
     </row>
     <row r="738">
       <c r="A738" s="0" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
     </row>
     <row r="739">
       <c r="A739" s="0" t="s">
-        <v>323</v>
+        <v>73</v>
       </c>
       <c r="B739" s="0" t="s">
-        <v>324</v>
+        <v>74</v>
       </c>
       <c r="C739" s="0" t="s">
-        <v>91</v>
+        <v>302</v>
       </c>
       <c r="D739" s="0" t="s">
-        <v>162</v>
+        <v>88</v>
       </c>
     </row>
     <row r="741">
       <c r="A741" s="0" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
     </row>
     <row r="742">
       <c r="A742" s="0" t="s">
-        <v>68</v>
+        <v>82</v>
       </c>
       <c r="B742" s="0" t="s">
-        <v>69</v>
+        <v>83</v>
       </c>
       <c r="C742" s="0" t="s">
-        <v>51</v>
+        <v>302</v>
       </c>
       <c r="D742" s="0" t="s">
         <v>88</v>
@@ -8295,128 +8396,242 @@
     </row>
     <row r="744">
       <c r="A744" s="0" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
     </row>
     <row r="745">
       <c r="A745" s="0" t="s">
-        <v>323</v>
+        <v>82</v>
       </c>
       <c r="B745" s="0" t="s">
-        <v>324</v>
+        <v>85</v>
       </c>
       <c r="C745" s="0" t="s">
-        <v>148</v>
+        <v>302</v>
       </c>
       <c r="D745" s="0" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="746">
-      <c r="A746" s="0" t="s">
-        <v>149</v>
-      </c>
-      <c r="B746" s="0" t="s">
-        <v>150</v>
-      </c>
-      <c r="C746" s="0" t="s">
-        <v>151</v>
-      </c>
-      <c r="D746" s="0" t="s">
-        <v>175</v>
+        <v>88</v>
       </c>
     </row>
     <row r="747">
       <c r="A747" s="0" t="s">
-        <v>149</v>
-      </c>
-      <c r="B747" s="0" t="s">
-        <v>152</v>
-      </c>
-      <c r="C747" s="0" t="s">
-        <v>153</v>
-      </c>
-      <c r="D747" s="0" t="s">
-        <v>175</v>
+        <v>345</v>
       </c>
     </row>
     <row r="748">
       <c r="A748" s="0" t="s">
-        <v>149</v>
+        <v>256</v>
       </c>
       <c r="B748" s="0" t="s">
-        <v>154</v>
+        <v>257</v>
       </c>
       <c r="C748" s="0" t="s">
-        <v>155</v>
+        <v>164</v>
       </c>
       <c r="D748" s="0" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="749">
-      <c r="A749" s="0" t="s">
-        <v>149</v>
-      </c>
-      <c r="B749" s="0" t="s">
-        <v>156</v>
-      </c>
-      <c r="C749" s="0" t="s">
-        <v>157</v>
-      </c>
-      <c r="D749" s="0" t="s">
-        <v>175</v>
+        <v>162</v>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" s="0" t="s">
+        <v>346</v>
       </c>
     </row>
     <row r="751">
       <c r="A751" s="0" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="752">
-      <c r="A752" s="0" t="s">
-        <v>323</v>
-      </c>
-      <c r="B752" s="0" t="s">
-        <v>324</v>
-      </c>
-      <c r="C752" s="0" t="s">
-        <v>350</v>
-      </c>
-      <c r="D752" s="0" t="s">
-        <v>162</v>
+        <v>307</v>
+      </c>
+      <c r="B751" s="0" t="s">
+        <v>308</v>
+      </c>
+      <c r="C751" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="D751" s="0" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="753">
       <c r="A753" s="0" t="s">
-        <v>323</v>
-      </c>
-      <c r="B753" s="0" t="s">
-        <v>324</v>
-      </c>
-      <c r="C753" s="0" t="s">
-        <v>258</v>
-      </c>
-      <c r="D753" s="0" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="755">
-      <c r="A755" s="0" t="s">
-        <v>351</v>
+        <v>347</v>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B754" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="C754" s="0" t="s">
+        <v>348</v>
+      </c>
+      <c r="D754" s="0" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="756">
       <c r="A756" s="0" t="s">
-        <v>323</v>
-      </c>
-      <c r="B756" s="0" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" s="0" t="s">
         <v>324</v>
       </c>
-      <c r="C756" s="0" t="s">
+      <c r="B757" s="0" t="s">
+        <v>325</v>
+      </c>
+      <c r="C757" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="D757" s="0" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" s="0" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="B760" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="C760" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="D756" s="0" t="s">
+      <c r="D760" s="0" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" s="0" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" s="0" t="s">
+        <v>324</v>
+      </c>
+      <c r="B763" s="0" t="s">
+        <v>325</v>
+      </c>
+      <c r="C763" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="D763" s="0" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="B764" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="C764" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="D764" s="0" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="B765" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="C765" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="D765" s="0" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="B766" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="C766" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="D766" s="0" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="B767" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="C767" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="D767" s="0" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" s="0" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" s="0" t="s">
+        <v>324</v>
+      </c>
+      <c r="B770" s="0" t="s">
+        <v>325</v>
+      </c>
+      <c r="C770" s="0" t="s">
+        <v>353</v>
+      </c>
+      <c r="D770" s="0" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" s="0" t="s">
+        <v>324</v>
+      </c>
+      <c r="B771" s="0" t="s">
+        <v>325</v>
+      </c>
+      <c r="C771" s="0" t="s">
+        <v>258</v>
+      </c>
+      <c r="D771" s="0" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" s="0" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" s="0" t="s">
+        <v>324</v>
+      </c>
+      <c r="B774" s="0" t="s">
+        <v>325</v>
+      </c>
+      <c r="C774" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="D774" s="0" t="s">
         <v>162</v>
       </c>
     </row>

</xml_diff>